<commit_message>
renaming files, misc cleanup
</commit_message>
<xml_diff>
--- a/CEA.xlsx
+++ b/CEA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B395F0C0-E6E7-A64E-8816-D26E7B07566C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E35F479-5BD8-5044-8833-7EEE7390661C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="17540" xr2:uid="{8DB7341E-9E79-1241-9245-6ACB3CE2C1AA}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="CEA" localSheetId="1">'CEA DATA'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -240,7 +240,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -274,11 +274,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,6 +912,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2141863168"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1860,26 +1861,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C946282-1CC7-CC4B-A68F-D39984492B33}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
       <c r="J1" t="s">
         <v>41</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -1950,11 +1951,11 @@
       <c r="H3">
         <v>2214.5</v>
       </c>
-      <c r="J3" s="3">
-        <f>F3-$C$17*$C$14/A3</f>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J10" si="0">F3-$C$17*$C$14/A3</f>
         <v>0.52942450000000008</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <f>E3*J3/$C$13</f>
         <v>81.017173638588631</v>
       </c>
@@ -1966,8 +1967,12 @@
         <f>$C$26/K3/$C$13</f>
         <v>0.15694203375596186</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <f>E3*F3</f>
+        <v>2214.5854799999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1992,24 +1997,28 @@
       <c r="H4">
         <v>2227</v>
       </c>
-      <c r="J4" s="3">
-        <f>F4-$C$17*$C$14/A4</f>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
         <v>1.0019122500000002</v>
       </c>
-      <c r="K4" s="4">
-        <f t="shared" ref="K4:K10" si="0">E4*J4/$C$13</f>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K10" si="1">E4*J4/$C$13</f>
         <v>154.2511649831736</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M10" si="1">$C$25/K4/$C$13</f>
+        <f t="shared" ref="M4:M10" si="2">$C$25/K4/$C$13</f>
         <v>0.16486099150547109</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N10" si="2">$C$26/K4/$C$13</f>
+        <f t="shared" ref="N4:N10" si="3">$C$26/K4/$C$13</f>
         <v>8.2430495752735547E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P4">
+        <f t="shared" ref="P4:P10" si="4">E4*F4</f>
+        <v>2226.95847</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -2034,24 +2043,28 @@
       <c r="H5">
         <v>2233.6</v>
       </c>
-      <c r="J5" s="3">
-        <f>F5-$C$17*$C$14/A5</f>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
         <v>1.1591415</v>
       </c>
-      <c r="K5" s="4">
-        <f t="shared" si="0"/>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
         <v>179.06052867632064</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.14201901551384685</v>
       </c>
       <c r="N5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1009507756923426E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <f t="shared" si="4"/>
+        <v>2233.72408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2076,24 +2089,28 @@
       <c r="H6">
         <v>2238</v>
       </c>
-      <c r="J6" s="3">
-        <f>F6-$C$17*$C$14/A6</f>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
         <v>1.2375061249999999</v>
       </c>
-      <c r="K6" s="4">
-        <f t="shared" si="0"/>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
         <v>191.59512532888027</v>
       </c>
       <c r="M6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.132727802736883</v>
       </c>
       <c r="N6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.6363901368441502E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>2237.9786199999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -2118,24 +2135,28 @@
       <c r="H7">
         <v>2241.3000000000002</v>
       </c>
-      <c r="J7" s="3">
-        <f>F7-$C$17*$C$14/A7</f>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
         <v>1.2845249000000001</v>
       </c>
-      <c r="K7" s="4">
-        <f t="shared" si="0"/>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
         <v>199.21532407913523</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12765082263399738</v>
       </c>
       <c r="N7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.382541131699869E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>2241.3550399999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2160,24 +2181,28 @@
       <c r="H8">
         <v>2243.8000000000002</v>
       </c>
-      <c r="J8" s="3">
-        <f>F8-$C$17*$C$14/A8</f>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
         <v>1.31567075</v>
       </c>
-      <c r="K8" s="4">
-        <f t="shared" si="0"/>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
         <v>204.31403407097696</v>
       </c>
       <c r="M8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12446526307226569</v>
       </c>
       <c r="N8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.2232631536132843E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>2243.6935199999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -2202,24 +2227,28 @@
       <c r="H9">
         <v>2245.9</v>
       </c>
-      <c r="J9" s="3">
-        <f>F9-$C$17*$C$14/A9</f>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
         <v>1.3380035000000001</v>
       </c>
-      <c r="K9" s="4">
-        <f t="shared" si="0"/>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
         <v>208.01410725576181</v>
       </c>
       <c r="M9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12225132389089736</v>
       </c>
       <c r="N9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.1125661945448682E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>2245.8933999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2244,29 +2273,33 @@
       <c r="H10">
         <v>2247.6</v>
       </c>
-      <c r="J10" s="3">
-        <f>F10-$C$17*$C$14/A10</f>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
         <v>1.3546030625000001</v>
       </c>
-      <c r="K10" s="4">
-        <f t="shared" si="0"/>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
         <v>210.78817184058232</v>
       </c>
       <c r="M10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12064244296986709</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.0321221484933546E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>2247.4981100000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2274,7 +2307,7 @@
         <v>9.8059999999999992</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2282,7 +2315,7 @@
         <v>0.101325</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>

</xml_diff>